<commit_message>
change to another system
</commit_message>
<xml_diff>
--- a/view/src/components/data/graph data.xlsx
+++ b/view/src/components/data/graph data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARINZE PC\Documents\My Project\Code\view\src\components\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARINZE PC\Documents\Projects\My Project\Code\view\src\components\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D2CB19-A83E-437D-B595-8E8B426C5477}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E3FCDC-FD42-4975-914A-5AA839E5FA43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A0AEB99F-6493-41B0-8424-9434ECCAE1BF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>from</t>
   </si>
@@ -76,15 +76,6 @@
   </si>
   <si>
     <t>GS</t>
-  </si>
-  <si>
-    <t>INE</t>
-  </si>
-  <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>MC</t>
   </si>
   <si>
     <t>FAG</t>
@@ -439,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89CD5CE-2AFF-448E-BD58-2F8D4CF20210}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +557,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -608,16 +599,16 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>447</v>
+        <v>862</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,16 +616,16 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>862</v>
+        <v>590</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,84 +633,84 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>590</v>
+        <v>403</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>403</v>
+        <v>310.16000000000003</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>474</v>
+        <v>810.51</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>328</v>
+        <v>538.84</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>693</v>
+        <v>83.04</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -727,16 +718,16 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>310.16000000000003</v>
+        <v>825</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -744,16 +735,16 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>810.51</v>
+        <v>832.35</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,16 +752,16 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>538.84</v>
+        <v>472.7</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -778,84 +769,84 @@
         <v>2</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>83.04</v>
+        <v>447.57</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>825</v>
+        <v>783.57</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C22">
-        <v>832.35</v>
+        <v>387.72</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>472.7</v>
+        <v>232.3</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>447.57</v>
+        <v>783.57</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -863,16 +854,16 @@
         <v>3</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>783.57</v>
+        <v>336.15</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -880,117 +871,32 @@
         <v>3</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C26">
-        <v>387.72</v>
+        <v>404.93</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>232.3</v>
+        <v>718.61</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28">
-        <v>7</v>
-      </c>
-      <c r="C28">
-        <v>783.57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>3</v>
-      </c>
-      <c r="B29">
-        <v>8</v>
-      </c>
-      <c r="C29">
-        <v>336.15</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>3</v>
-      </c>
-      <c r="B30">
-        <v>9</v>
-      </c>
-      <c r="C30">
-        <v>404.93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31">
-        <v>10</v>
-      </c>
-      <c r="C31">
-        <v>447.43</v>
-      </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32">
-        <v>11</v>
-      </c>
-      <c r="C32">
-        <v>718.61</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>